<commit_message>
Optimizasyon modellemesi matlab koduna başlandı. Parametreler tanıtıldı.
</commit_message>
<xml_diff>
--- a/Paper/PEMD 2018/Optimization Work/study/parameters.xlsx
+++ b/Paper/PEMD 2018/Optimization Work/study/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\IMMD\Paper\PEMD 2018\Optimization Work\study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mesutto\Desktop\github work\IMMD\Paper\PEMD 2018\Optimization Work\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,9 +80,6 @@
     <t>l</t>
   </si>
   <si>
-    <t>α, em, w, p</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Pout, Armst, Bgt, Jrmst, wr, Br, </t>
     </r>
@@ -179,7 +176,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Tm, kw, Qs, Eph, Iph, </t>
+      <t xml:space="preserve">Tm, kw, Qs, p, Eph, Iph, </t>
     </r>
     <r>
       <rPr>
@@ -213,11 +210,14 @@
       <t>αs, Lm, Plossm</t>
     </r>
   </si>
+  <si>
+    <t>α, em, w</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,13 +626,13 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -640,22 +640,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -666,14 +666,14 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -689,13 +689,13 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>